<commit_message>
new way to get games
</commit_message>
<xml_diff>
--- a/traders/checklist.xlsx
+++ b/traders/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/traders/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFFEBD5E-A7EE-7B4B-935A-B48E4575B428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC89212-12CF-0F49-B135-120ED54BDDD4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="26740" windowHeight="15780" xr2:uid="{83570033-C547-D34E-9F9C-D9B045508882}"/>
   </bookViews>
@@ -83,10 +83,10 @@
     <t>トレイダーズ! スーパーシナリオサポート 11</t>
   </si>
   <si>
-    <t>Traders! Super Session Support 7</t>
-  </si>
-  <si>
     <t>Traders! Super Session Support 11</t>
+  </si>
+  <si>
+    <t>Traders! Super Session Support 6</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>